<commit_message>
starting new specific aims outline
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCCFD56-0A83-6641-8F38-57016C05DDB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE51920-ABA1-C94E-A85D-295DB7980368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39160" yWindow="5000" windowWidth="28040" windowHeight="16600" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
   <si>
     <t>Drafted</t>
   </si>
@@ -96,15 +96,6 @@
     <t>Description of Institutional Environment and Commitment to Training Note</t>
   </si>
   <si>
-    <t>From OSP</t>
-  </si>
-  <si>
-    <t>1. Cover Letter</t>
-  </si>
-  <si>
-    <t>With me</t>
-  </si>
-  <si>
     <t>Facilities</t>
   </si>
   <si>
@@ -112,13 +103,154 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Bibliography and references cited</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Technical description with long term goals and health relevance</t>
+  </si>
+  <si>
+    <t>Health relevance and creation of fundamental knoledge</t>
+  </si>
+  <si>
+    <t>No URLs - PMC number required for my papers can replace with URL to free full text if no PMCID</t>
+  </si>
+  <si>
+    <t>Cover Letter</t>
+  </si>
+  <si>
+    <t>Draft location</t>
+  </si>
+  <si>
+    <t>../../.git/modules/Fellowships/annex/objects/Gx/M1/SHA256E-s358400--a0d42f49c1c73dc8c0d7cc3d4052890be08d490fc4757830ff0f7e5baabbbced.doc/SHA256E-s358400--a0d42f49c1c73dc8c0d7cc3d4052890be08d490fc4757830ff0f7e5baabbbced.doc</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>template from OSP</t>
+  </si>
+  <si>
+    <t>Project_summary_abstract.docx</t>
+  </si>
+  <si>
+    <t>instructions from guide</t>
+  </si>
+  <si>
+    <t>project_narrative.docx</t>
+  </si>
+  <si>
+    <t>Description of location and how it will contribute to project success</t>
+  </si>
+  <si>
+    <t>facilities_and_other_resources.docx</t>
+  </si>
+  <si>
+    <t>List major items of equipment already available for this project and, if appropriate, identify the equipment's location and pertinent capabilities.</t>
+  </si>
+  <si>
+    <t>list_of_equiptment.docx</t>
+  </si>
+  <si>
+    <t>Special format CV basically</t>
+  </si>
+  <si>
+    <t>Biosketch_draft.docx</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>draft, should polish</t>
+  </si>
+  <si>
+    <t>My background and a breakdown of project percent effort by year</t>
+  </si>
+  <si>
+    <t>Applicant_Background_and_Goals_for_Fellowship_Training.docx</t>
+  </si>
+  <si>
+    <t>Goals of the project</t>
+  </si>
+  <si>
+    <t>F32_specific_aims.docx</t>
+  </si>
+  <si>
+    <t>Needs total rewrite</t>
+  </si>
+  <si>
+    <t>detailed description of the significance and experimental plan</t>
+  </si>
+  <si>
+    <t>/Users/jackdesmarais/Documents/Kinney_lab/.git/modules/Fellowships/annex/objects/G4/6f/SHA256E-s294879--ead2ff632e143486bce173f304f6f4e4089eaba7fe536b7f69f6ae3a35ba0b58.docx/SHA256E-s294879--ead2ff632e143486bce173f304f6f4e4089eaba7fe536b7f69f6ae3a35ba0b58.docx</t>
+  </si>
+  <si>
+    <t>description of my and Justin's contributions to the research plan</t>
+  </si>
+  <si>
+    <t>respective_contributions.docx</t>
+  </si>
+  <si>
+    <t>Explain why the sponsor and institution were selected to accomplish the research training goals. </t>
+  </si>
+  <si>
+    <t>selection_of_sponsor_and_institution.docx</t>
+  </si>
+  <si>
+    <t>describe my training in RCR and plan to get more</t>
+  </si>
+  <si>
+    <t>RCR_Template_2022.docx</t>
+  </si>
+  <si>
+    <t>Justin's previous work and success rate for these sorts of things</t>
+  </si>
+  <si>
+    <t>From Justin</t>
+  </si>
+  <si>
+    <t>Ask for letters from Peter and Adrian</t>
+  </si>
+  <si>
+    <t>Need to request</t>
+  </si>
+  <si>
+    <t>Show CSHL has an established history of this kind of research and a good environment for training me</t>
+  </si>
+  <si>
+    <t>F32 Institutional Environment and Commitment template_2022.docx</t>
+  </si>
+  <si>
+    <t>Resource sharing plan</t>
+  </si>
+  <si>
+    <t>describe how we will share resources we generate</t>
+  </si>
+  <si>
+    <t>resource_sharing_plan.docx</t>
+  </si>
+  <si>
+    <t>Authentication of key resources</t>
+  </si>
+  <si>
+    <t>describe how we will authenticate cell lines and reagents</t>
+  </si>
+  <si>
+    <t>Authentication_of_Key_Biological_Chemical_Resources.docx</t>
+  </si>
+  <si>
+    <t>Needs total rewrite (initial outline done)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,6 +270,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -156,18 +296,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -181,13 +331,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9D1F721-3EBE-0345-9CBA-2847C15A969F}" name="Table1" displayName="Table1" ref="A1:D17" totalsRowShown="0">
-  <autoFilter ref="A1:D17" xr:uid="{F9D1F721-3EBE-0345-9CBA-2847C15A969F}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9D1F721-3EBE-0345-9CBA-2847C15A969F}" name="Table1" displayName="Table1" ref="A1:F20" totalsRowShown="0">
+  <autoFilter ref="A1:F20" xr:uid="{F9D1F721-3EBE-0345-9CBA-2847C15A969F}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{924DD312-80E3-224B-846B-36D22BCE72F7}" name="Section of Application"/>
     <tableColumn id="2" xr3:uid="{6EC5F282-D866-A543-8965-2A4B2374BA62}" name="Page Limits"/>
+    <tableColumn id="5" xr3:uid="{A7F4C676-62EF-2E42-9856-07ADCFAC67FF}" name="Notes"/>
+    <tableColumn id="6" xr3:uid="{15D78AD3-33BD-BA49-9E49-FD80474C3096}" name="Draft location"/>
     <tableColumn id="3" xr3:uid="{4F62D0C8-A292-A94B-A0A8-4C9D0FA01AB9}" name="Drafted"/>
-    <tableColumn id="4" xr3:uid="{8288742E-9B0B-5946-AA65-19C0B01E20B5}" name="Current state"/>
+    <tableColumn id="4" xr3:uid="{8288742E-9B0B-5946-AA65-19C0B01E20B5}" name="Current state" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -490,20 +642,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A7C2F5-51DA-C347-BCB0-CFA75EBC1137}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="67" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -511,176 +666,410 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>6</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
       </c>
       <c r="B9">
         <v>6</v>
       </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B20">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>5</v>
-      </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F20" s="4"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{7C85B03E-64AE-5541-957F-2BAD2C2EAA18}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{2FEB8A65-9916-F148-894C-25FB7157652A}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{F185D559-5771-4F4B-9461-A25113C60547}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{5DE7D153-3E87-E44D-B056-B30740FCA201}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{0C6A06E6-570C-0341-940B-9A1C45D770DF}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{57BD57DC-58CF-1946-A624-66E1DC2E4DFF}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{EE421526-6E86-424E-A327-A031E911930B}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{A5EEF808-3394-1949-A06C-D738663F5A5B}"/>
+    <hyperlink ref="D11" r:id="rId9" display="/Users/jackdesmarais/Documents/Kinney_lab/.git/modules/Fellowships/annex/objects/G4/6f/SHA256E-s294879--ead2ff632e143486bce173f304f6f4e4089eaba7fe536b7f69f6ae3a35ba0b58.docx/SHA256E-s294879--ead2ff632e143486bce173f304f6f4e4089eaba7fe536b7f69f6ae3a35ba0b58.docx" xr:uid="{37BBACF5-57A2-514B-939C-56E3E1191F7C}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{B7DEA793-AFF1-7546-BEF4-AF0C238DB0B6}"/>
+    <hyperlink ref="D13" r:id="rId11" xr:uid="{6AE776CC-3D87-1347-AB0E-FD4C5AFA5F64}"/>
+    <hyperlink ref="D14" r:id="rId12" xr:uid="{E8D7CE4C-420C-3C41-86E7-D7617D6FAD0F}"/>
+    <hyperlink ref="D17" r:id="rId13" xr:uid="{8838A003-7D07-A24E-A587-7A7E1D4A15CD}"/>
+    <hyperlink ref="D18" r:id="rId14" xr:uid="{0CD94DE2-A612-8047-8F9E-9109DA81FD7F}"/>
+    <hyperlink ref="D19" r:id="rId15" xr:uid="{6A4BCA20-A8A7-9444-9854-58F036876127}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
starting redraft of specific aims
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE51920-ABA1-C94E-A85D-295DB7980368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361E5968-178E-3540-B496-43BB5BB97F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
@@ -243,7 +243,7 @@
     <t>Authentication_of_Key_Biological_Chemical_Resources.docx</t>
   </si>
   <si>
-    <t>Needs total rewrite (initial outline done)</t>
+    <t>Needs total rewrite (initial outline done, redraft started)</t>
   </si>
 </sst>
 </file>
@@ -645,7 +645,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -824,7 +824,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
adding some work on institutional env
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02E9E9F-EB5E-C643-B965-BA450B8E462F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D25AADA-C742-F049-8BC1-049BBE8A49C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
   <si>
     <t>Drafted</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>Finished</t>
+  </si>
+  <si>
+    <t>started</t>
+  </si>
+  <si>
+    <t>template from OSP (started)</t>
   </si>
 </sst>
 </file>
@@ -652,7 +658,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -983,7 +989,7 @@
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -997,10 +1003,10 @@
         <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="G17" s="4"/>
     </row>

</xml_diff>

<commit_message>
initial drafting of equiptment attatchment
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D25AADA-C742-F049-8BC1-049BBE8A49C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64985CB0-91A8-2C46-AF8F-E36E046CCE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
   <si>
     <t>Drafted</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>template from OSP (started)</t>
+  </si>
+  <si>
+    <t>Rough drafted, Needs model details</t>
   </si>
 </sst>
 </file>
@@ -658,7 +661,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -785,7 +788,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -799,10 +802,10 @@
         <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="G7" s="4"/>
     </row>

</xml_diff>

<commit_message>
began work on the RCR attatchment
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64985CB0-91A8-2C46-AF8F-E36E046CCE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDA1F5D-42E8-4F47-94B2-8B445BA513B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
   <si>
     <t>Drafted</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>Rough drafted, Needs model details</t>
+  </si>
+  <si>
+    <t>Started</t>
   </si>
 </sst>
 </file>
@@ -661,7 +664,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -935,7 +938,7 @@
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -949,10 +952,10 @@
         <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="G14" s="4"/>
     </row>

</xml_diff>

<commit_message>
first draft of specific aims sent to Justin
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDA1F5D-42E8-4F47-94B2-8B445BA513B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80F4E51-C29C-4041-BD1D-34676BFEC080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
+    <workbookView xWindow="28800" yWindow="1640" windowWidth="28800" windowHeight="16440" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
   <si>
     <t>Drafted</t>
   </si>
@@ -243,9 +243,6 @@
     <t>Authentication_of_Key_Biological_Chemical_Resources.docx</t>
   </si>
   <si>
-    <t>First draft done</t>
-  </si>
-  <si>
     <t>Finished</t>
   </si>
   <si>
@@ -259,6 +256,12 @@
   </si>
   <si>
     <t>Started</t>
+  </si>
+  <si>
+    <t>Waiting for update on RCR training date to complete. Need to decide if I should include CSHL policies on trainings not applicable to my proposal. Maybe can consolidate these.</t>
+  </si>
+  <si>
+    <t>Draft 1 Sent to Justin</t>
   </si>
 </sst>
 </file>
@@ -664,7 +667,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,7 +700,7 @@
         <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -808,7 +811,7 @@
         <v>41</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -871,7 +874,7 @@
         <v>41</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -938,7 +941,7 @@
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -952,10 +955,10 @@
         <v>55</v>
       </c>
       <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="G14" s="4"/>
     </row>
@@ -1009,10 +1012,10 @@
         <v>61</v>
       </c>
       <c r="E17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="G17" s="4"/>
     </row>

</xml_diff>

<commit_message>
drafting resource sharing plan
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80F4E51-C29C-4041-BD1D-34676BFEC080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D7BEF8-64B4-884B-9B72-935BE3C11916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="1640" windowWidth="28800" windowHeight="16440" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="76">
   <si>
     <t>Drafted</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>Draft 1 Sent to Justin</t>
+  </si>
+  <si>
+    <t>First draft created. Waiting on addgene for variant library submission guidelines</t>
   </si>
 </sst>
 </file>
@@ -667,7 +670,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1019,7 +1022,7 @@
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -1033,10 +1036,10 @@
         <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="G18" s="4"/>
     </row>

</xml_diff>

<commit_message>
first draft of authentication plan
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040C10E9-5BCC-A947-B555-E4CB686A2552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD0F4D0-4158-4049-8E08-7221E3D0031B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="1640" windowWidth="28800" windowHeight="16440" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
   <si>
     <t>Drafted</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>First draft created. Waiting on addgene for variant library submission guidelines</t>
+  </si>
+  <si>
+    <t>First draft done, waiting for justin to send his RO1 plan</t>
   </si>
 </sst>
 </file>
@@ -669,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A7C2F5-51DA-C347-BCB0-CFA75EBC1137}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E20" sqref="E19:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1043,7 +1046,7 @@
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1057,10 +1060,10 @@
         <v>67</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="G19" s="4"/>
     </row>

</xml_diff>

<commit_message>
starting to adapt facilities and resources from Justin's draft
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD0F4D0-4158-4049-8E08-7221E3D0031B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3AE2E7-A590-D34E-B040-5885D026C282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="1640" windowWidth="28800" windowHeight="16440" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="78">
   <si>
     <t>Drafted</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>First draft done, waiting for justin to send his RO1 plan</t>
+  </si>
+  <si>
+    <t>Adapted from Justin's still needs a lot of checking for asccuracy over elzar stats</t>
   </si>
 </sst>
 </file>
@@ -672,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A7C2F5-51DA-C347-BCB0-CFA75EBC1137}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E20" sqref="E19:E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -779,7 +782,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -793,10 +796,10 @@
         <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="G6" s="4"/>
     </row>

</xml_diff>

<commit_message>
Updated authentication with Justin's draft
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3AE2E7-A590-D34E-B040-5885D026C282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2A2450-2BA1-C743-B1C7-8E0BBB0A8ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="1640" windowWidth="28800" windowHeight="16440" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
@@ -243,6 +243,9 @@
     <t>Authentication_of_Key_Biological_Chemical_Resources.docx</t>
   </si>
   <si>
+    <t>First draft done</t>
+  </si>
+  <si>
     <t>Finished</t>
   </si>
   <si>
@@ -265,9 +268,6 @@
   </si>
   <si>
     <t>First draft created. Waiting on addgene for variant library submission guidelines</t>
-  </si>
-  <si>
-    <t>First draft done, waiting for justin to send his RO1 plan</t>
   </si>
   <si>
     <t>Adapted from Justin's still needs a lot of checking for asccuracy over elzar stats</t>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A7C2F5-51DA-C347-BCB0-CFA75EBC1137}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,7 +709,7 @@
         <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -796,7 +796,7 @@
         <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>77</v>
@@ -820,7 +820,7 @@
         <v>41</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -883,7 +883,7 @@
         <v>41</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -964,10 +964,10 @@
         <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G14" s="4"/>
     </row>
@@ -1021,10 +1021,10 @@
         <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G17" s="4"/>
     </row>
@@ -1045,11 +1045,11 @@
         <v>41</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>41</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G19" s="4"/>
     </row>

</xml_diff>

<commit_message>
updating equiptment list with info from Justin's RO1
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2A2450-2BA1-C743-B1C7-8E0BBB0A8ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3A8BE7-5FBE-AC4A-9959-3508386066FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="1640" windowWidth="28800" windowHeight="16440" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
@@ -255,9 +255,6 @@
     <t>template from OSP (started)</t>
   </si>
   <si>
-    <t>Rough drafted, Needs model details</t>
-  </si>
-  <si>
     <t>Started</t>
   </si>
   <si>
@@ -271,6 +268,9 @@
   </si>
   <si>
     <t>Adapted from Justin's still needs a lot of checking for asccuracy over elzar stats</t>
+  </si>
+  <si>
+    <t>Updated from Justin's</t>
   </si>
 </sst>
 </file>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A7C2F5-51DA-C347-BCB0-CFA75EBC1137}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,14 +796,14 @@
         <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -820,7 +820,7 @@
         <v>41</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -883,7 +883,7 @@
         <v>41</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -964,10 +964,10 @@
         <v>55</v>
       </c>
       <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="G14" s="4"/>
     </row>
@@ -1045,7 +1045,7 @@
         <v>41</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G18" s="4"/>
     </row>

</xml_diff>

<commit_message>
Updated resource sharing plan with info from Justin's RO1
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3A8BE7-5FBE-AC4A-9959-3508386066FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5638C7B7-EFB4-2548-A871-EFE4574A4F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="1640" windowWidth="28800" windowHeight="16440" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
@@ -264,13 +264,13 @@
     <t>Draft 1 Sent to Justin</t>
   </si>
   <si>
-    <t>First draft created. Waiting on addgene for variant library submission guidelines</t>
-  </si>
-  <si>
     <t>Adapted from Justin's still needs a lot of checking for asccuracy over elzar stats</t>
   </si>
   <si>
     <t>Updated from Justin's</t>
+  </si>
+  <si>
+    <t>Justin's RO1 incorporated</t>
   </si>
 </sst>
 </file>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A7C2F5-51DA-C347-BCB0-CFA75EBC1137}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -799,7 +799,7 @@
         <v>72</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -820,7 +820,7 @@
         <v>41</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>41</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G18" s="4"/>
     </row>

</xml_diff>

<commit_message>
adding Justins SA feedback
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5638C7B7-EFB4-2548-A871-EFE4574A4F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C54EDE-A4EB-E64B-A9AC-511CA9EAB60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="1640" windowWidth="28800" windowHeight="16440" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
   <si>
     <t>Drafted</t>
   </si>
@@ -261,9 +261,6 @@
     <t>Waiting for update on RCR training date to complete. Need to decide if I should include CSHL policies on trainings not applicable to my proposal. Maybe can consolidate these.</t>
   </si>
   <si>
-    <t>Draft 1 Sent to Justin</t>
-  </si>
-  <si>
     <t>Adapted from Justin's still needs a lot of checking for asccuracy over elzar stats</t>
   </si>
   <si>
@@ -271,6 +268,15 @@
   </si>
   <si>
     <t>Justin's RO1 incorporated</t>
+  </si>
+  <si>
+    <t>Comments back!</t>
+  </si>
+  <si>
+    <t>Needs rewrite</t>
+  </si>
+  <si>
+    <t>Needs polish</t>
   </si>
 </sst>
 </file>
@@ -676,7 +682,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -799,7 +805,7 @@
         <v>72</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -820,7 +826,7 @@
         <v>41</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -838,7 +844,7 @@
         <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>42</v>
@@ -859,7 +865,7 @@
         <v>44</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>42</v>
@@ -880,10 +886,10 @@
         <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -1045,7 +1051,7 @@
         <v>41</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G18" s="4"/>
     </row>

</xml_diff>

<commit_message>
implementing comments to the specific aims
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C54EDE-A4EB-E64B-A9AC-511CA9EAB60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54B7C29-ACDC-D140-AAAE-E12E4CA91B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="1640" windowWidth="28800" windowHeight="16440" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
@@ -270,13 +270,13 @@
     <t>Justin's RO1 incorporated</t>
   </si>
   <si>
-    <t>Comments back!</t>
-  </si>
-  <si>
-    <t>Needs rewrite</t>
-  </si>
-  <si>
     <t>Needs polish</t>
+  </si>
+  <si>
+    <t>Needs cutting</t>
+  </si>
+  <si>
+    <t>Comments in editing for length now</t>
   </si>
 </sst>
 </file>
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A7C2F5-51DA-C347-BCB0-CFA75EBC1137}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -844,7 +844,7 @@
         <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>42</v>
@@ -865,14 +865,14 @@
         <v>44</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>42</v>
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -889,7 +889,7 @@
         <v>78</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G10" s="4"/>
     </row>

</xml_diff>

<commit_message>
Cut new F32 to length
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54B7C29-ACDC-D140-AAAE-E12E4CA91B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6AE081-5FED-3F43-8586-D1AE3D1C0EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="1640" windowWidth="28800" windowHeight="16440" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
@@ -273,10 +273,10 @@
     <t>Needs polish</t>
   </si>
   <si>
-    <t>Needs cutting</t>
-  </si>
-  <si>
-    <t>Comments in editing for length now</t>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>One last read then send for comments.</t>
   </si>
 </sst>
 </file>
@@ -682,7 +682,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
cleaning up 2nd draft for specific aims
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6AE081-5FED-3F43-8586-D1AE3D1C0EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5106F0-5249-9548-897F-D78EBA8DCD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="1640" windowWidth="28800" windowHeight="16440" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -276,7 +276,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t>One last read then send for comments.</t>
+    <t>Resdy to return to Justin</t>
   </si>
 </sst>
 </file>
@@ -682,7 +682,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
begun writing the selection of sponsor and institution
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5106F0-5249-9548-897F-D78EBA8DCD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03040ED7-413A-314A-9804-CB45598B59EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="81">
   <si>
     <t>Drafted</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>Resdy to return to Justin</t>
+  </si>
+  <si>
+    <t>work begun</t>
   </si>
 </sst>
 </file>
@@ -682,7 +685,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -949,10 +952,10 @@
         <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="G13" s="4"/>
     </row>

</xml_diff>

<commit_message>
starting to put in edits from Justin meeting
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03040ED7-413A-314A-9804-CB45598B59EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF2D226-A5D3-F74D-8384-4691F9411FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
   <si>
     <t>Drafted</t>
   </si>
@@ -279,7 +279,10 @@
     <t>Resdy to return to Justin</t>
   </si>
   <si>
-    <t>work begun</t>
+    <t>First draft needs cutting and editing</t>
+  </si>
+  <si>
+    <t>Needs polish and cutting</t>
   </si>
 </sst>
 </file>
@@ -685,7 +688,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -938,7 +941,7 @@
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -952,7 +955,7 @@
         <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
justin round 2 comments in for specific aims. Needs cutting to length
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF2D226-A5D3-F74D-8384-4691F9411FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E22A16-8E0A-E549-A5C2-52CE38E46DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
+    <workbookView xWindow="28800" yWindow="1760" windowWidth="28800" windowHeight="16580" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -273,16 +273,16 @@
     <t>Needs polish</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Resdy to return to Justin</t>
-  </si>
-  <si>
     <t>First draft needs cutting and editing</t>
   </si>
   <si>
     <t>Needs polish and cutting</t>
+  </si>
+  <si>
+    <t>Needs cutting</t>
+  </si>
+  <si>
+    <t>Justin's round 2 comments in needs cutting to length.</t>
   </si>
 </sst>
 </file>
@@ -688,7 +688,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -878,7 +878,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -892,10 +892,10 @@
         <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -955,10 +955,10 @@
         <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G13" s="4"/>
     </row>

</xml_diff>

<commit_message>
recording SA resend in the workbook
</commit_message>
<xml_diff>
--- a/2023_08_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_08_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_08_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E22A16-8E0A-E549-A5C2-52CE38E46DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDF2C20-8AED-4D49-893C-0BB431EC65E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="1760" windowWidth="28800" windowHeight="16580" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="81">
   <si>
     <t>Drafted</t>
   </si>
@@ -279,10 +279,7 @@
     <t>Needs polish and cutting</t>
   </si>
   <si>
-    <t>Needs cutting</t>
-  </si>
-  <si>
-    <t>Justin's round 2 comments in needs cutting to length.</t>
+    <t>Sent back to Justin for more comments</t>
   </si>
 </sst>
 </file>
@@ -687,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A7C2F5-51DA-C347-BCB0-CFA75EBC1137}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -878,7 +875,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -892,10 +889,10 @@
         <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="G10" s="4"/>
     </row>

</xml_diff>